<commit_message>
ui and term wise excel
</commit_message>
<xml_diff>
--- a/iso_excel.xlsx
+++ b/iso_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nishantmaurya/Documents/mummy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426CE77E-C26D-ED4B-856A-A91490FFACDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF624F14-F566-9E4F-81E1-C42689BB7E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="26">
   <si>
     <t>SR.NO.</t>
   </si>
@@ -100,10 +100,19 @@
     <t>+</t>
   </si>
   <si>
-    <t>+ 1</t>
-  </si>
-  <si>
     <t>OD</t>
+  </si>
+  <si>
+    <t>NOV</t>
+  </si>
+  <si>
+    <t>DEC</t>
+  </si>
+  <si>
+    <t>JAN</t>
+  </si>
+  <si>
+    <t>FEB</t>
   </si>
 </sst>
 </file>
@@ -125,7 +134,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,12 +162,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -257,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -292,10 +295,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -309,10 +308,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -338,10 +333,6 @@
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
@@ -363,6 +354,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -675,8 +670,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AF11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="161" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="161" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AG3" sqref="AG3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -691,48 +686,48 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="29" t="s">
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="29" t="s">
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="29" t="s">
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="29" t="s">
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="30"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="29" t="s">
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="AC1" s="30"/>
-      <c r="AD1" s="30"/>
-      <c r="AE1" s="30"/>
-      <c r="AF1" s="31"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="29"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
@@ -794,7 +789,7 @@
       <c r="U2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="V2" s="11" t="s">
+      <c r="V2" s="10" t="s">
         <v>12</v>
       </c>
       <c r="W2" s="7" t="s">
@@ -809,22 +804,22 @@
       <c r="Z2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="11" t="s">
+      <c r="AA2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AB2" s="12" t="s">
+      <c r="AB2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="AC2" s="13" t="s">
+      <c r="AC2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="AD2" s="13" t="s">
+      <c r="AD2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AE2" s="14" t="s">
+      <c r="AE2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="AF2" s="15" t="s">
+      <c r="AF2" s="26" t="s">
         <v>12</v>
       </c>
     </row>
@@ -837,86 +832,86 @@
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="8"/>
-      <c r="E3" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="21" t="str">
+      <c r="E3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="19" t="str">
         <f t="shared" ref="F3:F9" si="0">SUBSTITUTE(TRIM(CONCATENATE(D3, "", E3)),"+ 0"," ")</f>
         <v>+</v>
       </c>
-      <c r="G3" s="22">
+      <c r="G3" s="20">
         <f>C3-D3</f>
         <v>0</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="8"/>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="21" t="str">
+      <c r="K3" s="19" t="str">
         <f t="shared" ref="K3:K9" si="1">SUBSTITUTE(TRIM(CONCATENATE(I3, "", J3)),"+ 0"," ")</f>
         <v>+</v>
       </c>
-      <c r="L3" s="22">
+      <c r="L3" s="20">
         <f>H3-I3</f>
         <v>0</v>
       </c>
       <c r="M3" s="7"/>
       <c r="N3" s="8"/>
-      <c r="O3" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="P3" s="21" t="str">
+      <c r="O3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="19" t="str">
         <f t="shared" ref="P3:P9" si="2">SUBSTITUTE(TRIM(CONCATENATE(N3, "", O3)),"+ 0"," ")</f>
         <v>+</v>
       </c>
-      <c r="Q3" s="22">
+      <c r="Q3" s="20">
         <f>M3-N3</f>
         <v>0</v>
       </c>
       <c r="R3" s="7"/>
       <c r="S3" s="8"/>
-      <c r="T3" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="U3" s="21" t="str">
+      <c r="T3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="U3" s="19" t="str">
         <f>SUBSTITUTE(TRIM(CONCATENATE(S3, "", T3)),"+ 0"," ")</f>
         <v>+</v>
       </c>
-      <c r="V3" s="23">
+      <c r="V3" s="20">
         <f>R3-S3</f>
         <v>0</v>
       </c>
       <c r="W3" s="7"/>
       <c r="X3" s="8"/>
-      <c r="Y3" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z3" s="21" t="str">
+      <c r="Y3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z3" s="19" t="str">
         <f t="shared" ref="Z3:Z9" si="3">SUBSTITUTE(TRIM(CONCATENATE(X3, "", Y3)),"+ 0"," ")</f>
         <v>+</v>
       </c>
-      <c r="AA3" s="23">
+      <c r="AA3" s="20">
         <f>W3-X3</f>
         <v>0</v>
       </c>
-      <c r="AB3" s="24">
+      <c r="AB3" s="21">
         <f t="shared" ref="AB3:AC9" si="4">C3+H3+M3+R3+W3</f>
         <v>0</v>
       </c>
-      <c r="AC3" s="25">
+      <c r="AC3" s="22">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AD3" s="25">
+      <c r="AD3" s="22">
         <f>IFERROR(VALUE(MID(E4,2,3)),0) + IFERROR(VALUE(MID(J4,2,3)),0) + IFERROR(VALUE(MID(O4,2,3)),0) + IFERROR(VALUE(MID(T4,2,3)),0) + IFERROR(VALUE(MID(Y4,2,3)),0)</f>
         <v>0</v>
       </c>
-      <c r="AE3" s="21" t="str">
+      <c r="AE3" s="19" t="str">
         <f>CONCATENATE(MID(AC3,1,3)," + ", MID(AD3,1,2))</f>
         <v>0 + 0</v>
       </c>
-      <c r="AF3" s="23">
+      <c r="AF3" s="20">
         <f>G3+L3+Q3+V3+AA3</f>
         <v>0</v>
       </c>
@@ -930,86 +925,86 @@
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="8"/>
-      <c r="E4" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="21" t="str">
+      <c r="E4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="19" t="str">
         <f t="shared" si="0"/>
         <v>+</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="20">
         <f>C4-D4</f>
         <v>0</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="8"/>
-      <c r="J4" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="21" t="str">
+      <c r="J4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="19" t="str">
         <f t="shared" si="1"/>
         <v>+</v>
       </c>
-      <c r="L4" s="22">
+      <c r="L4" s="20">
         <f>H4-I4</f>
         <v>0</v>
       </c>
       <c r="M4" s="7"/>
       <c r="N4" s="8"/>
-      <c r="O4" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="P4" s="21" t="str">
+      <c r="O4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P4" s="19" t="str">
         <f t="shared" si="2"/>
         <v>+</v>
       </c>
-      <c r="Q4" s="22">
+      <c r="Q4" s="20">
         <f>M4-N4</f>
         <v>0</v>
       </c>
       <c r="R4" s="7"/>
       <c r="S4" s="8"/>
-      <c r="T4" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="U4" s="21" t="str">
+      <c r="T4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="U4" s="19" t="str">
         <f>SUBSTITUTE(TRIM(CONCATENATE(S4, "", T4)),"+ 0"," ")</f>
         <v>+</v>
       </c>
-      <c r="V4" s="23">
+      <c r="V4" s="20">
         <f>R4-S4</f>
         <v>0</v>
       </c>
       <c r="W4" s="7"/>
       <c r="X4" s="8"/>
-      <c r="Y4" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z4" s="21" t="str">
+      <c r="Y4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z4" s="19" t="str">
         <f t="shared" si="3"/>
         <v>+</v>
       </c>
-      <c r="AA4" s="23">
+      <c r="AA4" s="20">
         <f>W4-X4</f>
         <v>0</v>
       </c>
-      <c r="AB4" s="24">
+      <c r="AB4" s="21">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AC4" s="25">
+      <c r="AC4" s="22">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AD4" s="25">
+      <c r="AD4" s="22">
         <f t="shared" ref="AD4:AD9" si="5">IFERROR(VALUE(MID(E5,2,3)),0) + IFERROR(VALUE(MID(J5,2,3)),0) + IFERROR(VALUE(MID(O5,2,3)),0) + IFERROR(VALUE(MID(T5,2,3)),0) + IFERROR(VALUE(MID(Y5,2,3)),0)</f>
         <v>0</v>
       </c>
-      <c r="AE4" s="21" t="str">
+      <c r="AE4" s="19" t="str">
         <f>CONCATENATE(MID(AC4,1,3)," + ", MID(AD4,1,2))</f>
         <v>0 + 0</v>
       </c>
-      <c r="AF4" s="23">
+      <c r="AF4" s="20">
         <f>G4+L4+Q4+V4+AA4</f>
         <v>0</v>
       </c>
@@ -1023,86 +1018,86 @@
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="21" t="str">
+      <c r="E5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="19" t="str">
         <f t="shared" si="0"/>
         <v>+</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="20">
         <f>C5-D5</f>
         <v>0</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="8"/>
-      <c r="J5" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" s="21" t="str">
+      <c r="J5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="19" t="str">
         <f t="shared" si="1"/>
         <v>+</v>
       </c>
-      <c r="L5" s="22">
+      <c r="L5" s="20">
         <f>H5-I5</f>
         <v>0</v>
       </c>
       <c r="M5" s="7"/>
       <c r="N5" s="8"/>
-      <c r="O5" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="P5" s="21" t="str">
+      <c r="O5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P5" s="19" t="str">
         <f t="shared" si="2"/>
         <v>+</v>
       </c>
-      <c r="Q5" s="22">
+      <c r="Q5" s="20">
         <f>M5-N5</f>
         <v>0</v>
       </c>
       <c r="R5" s="7"/>
       <c r="S5" s="8"/>
-      <c r="T5" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="U5" s="21" t="str">
+      <c r="T5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="U5" s="19" t="str">
         <f>SUBSTITUTE(TRIM(CONCATENATE(S5, "", T5)),"+ 0"," ")</f>
         <v>+</v>
       </c>
-      <c r="V5" s="23">
+      <c r="V5" s="20">
         <f>R5-S5</f>
         <v>0</v>
       </c>
       <c r="W5" s="7"/>
       <c r="X5" s="8"/>
-      <c r="Y5" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z5" s="21" t="str">
+      <c r="Y5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z5" s="19" t="str">
         <f t="shared" si="3"/>
         <v>+</v>
       </c>
-      <c r="AA5" s="23">
+      <c r="AA5" s="20">
         <f>W5-X5</f>
         <v>0</v>
       </c>
-      <c r="AB5" s="24">
+      <c r="AB5" s="21">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AC5" s="25">
+      <c r="AC5" s="22">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AD5" s="25">
+      <c r="AD5" s="22">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AE5" s="21" t="str">
+      <c r="AE5" s="19" t="str">
         <f>CONCATENATE(MID(AC5,1,3)," + ", MID(AD5,1,2))</f>
         <v>0 + 0</v>
       </c>
-      <c r="AF5" s="23">
+      <c r="AF5" s="20">
         <f>G5+L5+Q5+V5+AA5</f>
         <v>0</v>
       </c>
@@ -1116,86 +1111,86 @@
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="8"/>
-      <c r="E6" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="21" t="str">
+      <c r="E6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="19" t="str">
         <f t="shared" si="0"/>
         <v>+</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="20">
         <f>C6-D6</f>
         <v>0</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="8"/>
-      <c r="J6" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="K6" s="21" t="str">
+      <c r="J6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="19" t="str">
         <f t="shared" si="1"/>
         <v>+</v>
       </c>
-      <c r="L6" s="22">
+      <c r="L6" s="20">
         <f>H6-I6</f>
         <v>0</v>
       </c>
       <c r="M6" s="7"/>
       <c r="N6" s="8"/>
-      <c r="O6" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="P6" s="21" t="str">
+      <c r="O6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P6" s="19" t="str">
         <f t="shared" si="2"/>
         <v>+</v>
       </c>
-      <c r="Q6" s="22">
+      <c r="Q6" s="20">
         <f>M6-N6</f>
         <v>0</v>
       </c>
       <c r="R6" s="7"/>
       <c r="S6" s="8"/>
-      <c r="T6" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="U6" s="21" t="str">
+      <c r="T6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="U6" s="19" t="str">
         <f>SUBSTITUTE(TRIM(CONCATENATE(S6, "", T6)),"+ 0"," ")</f>
         <v>+</v>
       </c>
-      <c r="V6" s="23">
+      <c r="V6" s="20">
         <f>R6-S6</f>
         <v>0</v>
       </c>
       <c r="W6" s="7"/>
       <c r="X6" s="8"/>
-      <c r="Y6" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z6" s="21" t="str">
+      <c r="Y6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z6" s="19" t="str">
         <f t="shared" si="3"/>
         <v>+</v>
       </c>
-      <c r="AA6" s="23">
+      <c r="AA6" s="20">
         <f>W6-X6</f>
         <v>0</v>
       </c>
-      <c r="AB6" s="24">
+      <c r="AB6" s="21">
         <f>C6+H6+M6+R6+W6</f>
         <v>0</v>
       </c>
-      <c r="AC6" s="25">
+      <c r="AC6" s="22">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AD6" s="25">
+      <c r="AD6" s="22">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AE6" s="21" t="str">
+      <c r="AE6" s="19" t="str">
         <f>CONCATENATE(MID(AC6,1,3)," + ", MID(AD6,1,2))</f>
         <v>0 + 0</v>
       </c>
-      <c r="AF6" s="23">
+      <c r="AF6" s="20">
         <f>G6+L6+Q6+V6+AA6</f>
         <v>0</v>
       </c>
@@ -1209,86 +1204,86 @@
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="21" t="str">
+      <c r="E7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="19" t="str">
         <f t="shared" si="0"/>
         <v>+</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="20">
         <f>C7-D7</f>
         <v>0</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="8"/>
-      <c r="J7" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="21" t="str">
+      <c r="J7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="19" t="str">
         <f t="shared" si="1"/>
         <v>+</v>
       </c>
-      <c r="L7" s="22">
+      <c r="L7" s="20">
         <f>H7-I7</f>
         <v>0</v>
       </c>
       <c r="M7" s="7"/>
       <c r="N7" s="8"/>
-      <c r="O7" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="P7" s="21" t="str">
+      <c r="O7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P7" s="19" t="str">
         <f t="shared" si="2"/>
         <v>+</v>
       </c>
-      <c r="Q7" s="22">
+      <c r="Q7" s="20">
         <f>M7-N7</f>
         <v>0</v>
       </c>
       <c r="R7" s="7"/>
       <c r="S7" s="8"/>
-      <c r="T7" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="U7" s="21" t="str">
+      <c r="T7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="U7" s="19" t="str">
         <f>SUBSTITUTE(TRIM(CONCATENATE(S7, "", T7)),"+ 0"," ")</f>
         <v>+</v>
       </c>
-      <c r="V7" s="23">
+      <c r="V7" s="20">
         <f>R7-S7</f>
         <v>0</v>
       </c>
       <c r="W7" s="7"/>
       <c r="X7" s="8"/>
-      <c r="Y7" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z7" s="21" t="str">
+      <c r="Y7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z7" s="19" t="str">
         <f t="shared" si="3"/>
         <v>+</v>
       </c>
-      <c r="AA7" s="23">
+      <c r="AA7" s="20">
         <f>W7-X7</f>
         <v>0</v>
       </c>
-      <c r="AB7" s="24">
+      <c r="AB7" s="21">
         <f>C7+H7+M7+R7+W7</f>
         <v>0</v>
       </c>
-      <c r="AC7" s="25">
+      <c r="AC7" s="22">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AD7" s="25">
+      <c r="AD7" s="22">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AE7" s="21" t="str">
+      <c r="AE7" s="19" t="str">
         <f>CONCATENATE(MID(AC7,1,3)," + ", MID(AD7,1,2))</f>
         <v>0 + 0</v>
       </c>
-      <c r="AF7" s="23">
+      <c r="AF7" s="20">
         <f>G7+L7+Q7+V7+AA7</f>
         <v>0</v>
       </c>
@@ -1302,86 +1297,86 @@
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="8"/>
-      <c r="E8" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="21" t="str">
+      <c r="E8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="19" t="str">
         <f t="shared" si="0"/>
         <v>+</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G8" s="20">
         <f t="shared" ref="G8:G9" si="6">C8-D8</f>
         <v>0</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="8"/>
-      <c r="J8" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" s="21" t="str">
+      <c r="J8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="19" t="str">
         <f t="shared" si="1"/>
         <v>+</v>
       </c>
-      <c r="L8" s="22">
+      <c r="L8" s="20">
         <f t="shared" ref="L8:L9" si="7">H8-I8</f>
         <v>0</v>
       </c>
       <c r="M8" s="7"/>
       <c r="N8" s="8"/>
-      <c r="O8" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="P8" s="21" t="str">
+      <c r="O8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P8" s="19" t="str">
         <f t="shared" si="2"/>
         <v>+</v>
       </c>
-      <c r="Q8" s="22">
+      <c r="Q8" s="20">
         <f t="shared" ref="Q8:Q9" si="8">M8-N8</f>
         <v>0</v>
       </c>
       <c r="R8" s="7"/>
       <c r="S8" s="8"/>
-      <c r="T8" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="U8" s="21" t="str">
+      <c r="T8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="U8" s="19" t="str">
         <f t="shared" ref="U8:U9" si="9">SUBSTITUTE(TRIM(CONCATENATE(S8, "", T8)),"+ 0"," ")</f>
         <v>+</v>
       </c>
-      <c r="V8" s="23">
+      <c r="V8" s="20">
         <f t="shared" ref="V8:V9" si="10">R8-S8</f>
         <v>0</v>
       </c>
       <c r="W8" s="7"/>
       <c r="X8" s="8"/>
-      <c r="Y8" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z8" s="21" t="str">
+      <c r="Y8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z8" s="19" t="str">
         <f t="shared" si="3"/>
         <v>+</v>
       </c>
-      <c r="AA8" s="23">
+      <c r="AA8" s="20">
         <f t="shared" ref="AA8:AA11" si="11">W8-X8</f>
         <v>0</v>
       </c>
-      <c r="AB8" s="24">
+      <c r="AB8" s="21">
         <f t="shared" ref="AB8:AC11" si="12">C8+H8+M8+R8+W8</f>
         <v>0</v>
       </c>
-      <c r="AC8" s="25">
+      <c r="AC8" s="22">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AD8" s="25">
+      <c r="AD8" s="22">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AE8" s="21" t="str">
+      <c r="AE8" s="19" t="str">
         <f t="shared" ref="AE8:AE9" si="13">CONCATENATE(MID(AC8,1,3)," + ", MID(AD8,1,2))</f>
         <v>0 + 0</v>
       </c>
-      <c r="AF8" s="23">
+      <c r="AF8" s="20">
         <f t="shared" ref="AF8:AF11" si="14">G8+L8+Q8+V8+AA8</f>
         <v>0</v>
       </c>
@@ -1391,90 +1386,90 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="21" t="str">
+      <c r="E9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="19" t="str">
         <f t="shared" si="0"/>
         <v>+</v>
       </c>
-      <c r="G9" s="22">
+      <c r="G9" s="20">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="8"/>
-      <c r="J9" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="K9" s="21" t="str">
+      <c r="J9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="19" t="str">
         <f t="shared" si="1"/>
         <v>+</v>
       </c>
-      <c r="L9" s="22">
+      <c r="L9" s="20">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M9" s="7"/>
       <c r="N9" s="8"/>
-      <c r="O9" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="P9" s="21" t="str">
+      <c r="O9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P9" s="19" t="str">
         <f t="shared" si="2"/>
         <v>+</v>
       </c>
-      <c r="Q9" s="22">
+      <c r="Q9" s="20">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="R9" s="7"/>
       <c r="S9" s="8"/>
-      <c r="T9" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="U9" s="21" t="str">
+      <c r="T9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="U9" s="19" t="str">
         <f t="shared" si="9"/>
         <v>+</v>
       </c>
-      <c r="V9" s="23">
+      <c r="V9" s="20">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="W9" s="7"/>
       <c r="X9" s="8"/>
-      <c r="Y9" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z9" s="21" t="str">
+      <c r="Y9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z9" s="19" t="str">
         <f t="shared" si="3"/>
         <v>+</v>
       </c>
-      <c r="AA9" s="23">
+      <c r="AA9" s="20">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AB9" s="24">
+      <c r="AB9" s="21">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AC9" s="25">
+      <c r="AC9" s="22">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AD9" s="25">
+      <c r="AD9" s="22">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AE9" s="21" t="str">
+      <c r="AE9" s="19" t="str">
         <f t="shared" si="13"/>
         <v>0 + 0</v>
       </c>
-      <c r="AF9" s="23">
+      <c r="AF9" s="20">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -1484,137 +1479,137 @@
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="16"/>
+      <c r="E10" s="14"/>
       <c r="F10" s="9"/>
       <c r="G10" s="10"/>
       <c r="H10" s="7"/>
       <c r="I10" s="8"/>
-      <c r="J10" s="16"/>
+      <c r="J10" s="14"/>
       <c r="K10" s="9"/>
       <c r="L10" s="10"/>
       <c r="M10" s="7"/>
       <c r="N10" s="8"/>
-      <c r="O10" s="16"/>
+      <c r="O10" s="14"/>
       <c r="P10" s="9"/>
       <c r="Q10" s="10"/>
       <c r="R10" s="7"/>
       <c r="S10" s="8"/>
-      <c r="T10" s="16"/>
+      <c r="T10" s="14"/>
       <c r="U10" s="9"/>
-      <c r="V10" s="11"/>
+      <c r="V10" s="10"/>
       <c r="W10" s="7"/>
       <c r="X10" s="8"/>
-      <c r="Y10" s="16"/>
+      <c r="Y10" s="14"/>
       <c r="Z10" s="9"/>
-      <c r="AA10" s="11"/>
-      <c r="AB10" s="17"/>
+      <c r="AA10" s="10"/>
+      <c r="AB10" s="15"/>
       <c r="AC10" s="8"/>
       <c r="AD10" s="8"/>
       <c r="AE10" s="9"/>
-      <c r="AF10" s="11"/>
+      <c r="AF10" s="10"/>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="26">
+      <c r="B11" s="17"/>
+      <c r="C11" s="23">
         <f>SUM(C3:C9)</f>
         <v>0</v>
       </c>
       <c r="D11" s="3"/>
-      <c r="E11" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="27" t="str">
+      <c r="E11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="24" t="str">
         <f t="shared" ref="F11" si="15">CONCATENATE(D11, " ", E11)</f>
         <v xml:space="preserve"> + </v>
       </c>
-      <c r="G11" s="26">
+      <c r="G11" s="23">
         <f>C11-D11</f>
         <v>0</v>
       </c>
-      <c r="H11" s="26">
+      <c r="H11" s="23">
         <f>SUM(H3:H9)</f>
         <v>0</v>
       </c>
       <c r="I11" s="3"/>
-      <c r="J11" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="27" t="str">
+      <c r="J11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="24" t="str">
         <f t="shared" ref="K11" si="16">CONCATENATE(I11, " ", J11)</f>
         <v xml:space="preserve"> + </v>
       </c>
-      <c r="L11" s="26">
+      <c r="L11" s="23">
         <f t="shared" ref="L11" si="17">H11-I11</f>
         <v>0</v>
       </c>
-      <c r="M11" s="26">
+      <c r="M11" s="23">
         <f>SUM(M3:M9)</f>
         <v>0</v>
       </c>
       <c r="N11" s="3"/>
-      <c r="O11" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="P11" s="27" t="str">
+      <c r="O11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="P11" s="24" t="str">
         <f t="shared" ref="P11" si="18">CONCATENATE(N11, " ", O11)</f>
         <v xml:space="preserve"> + </v>
       </c>
-      <c r="Q11" s="26">
+      <c r="Q11" s="23">
         <f t="shared" ref="Q11" si="19">M11-N11</f>
         <v>0</v>
       </c>
-      <c r="R11" s="26">
+      <c r="R11" s="23">
         <f>SUM(R3:R9)</f>
         <v>0</v>
       </c>
       <c r="S11" s="3"/>
-      <c r="T11" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="U11" s="27" t="str">
+      <c r="T11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="U11" s="24" t="str">
         <f t="shared" ref="U11" si="20">CONCATENATE(S11, "", T11)</f>
         <v xml:space="preserve">+ </v>
       </c>
-      <c r="V11" s="26">
+      <c r="V11" s="23">
         <f t="shared" ref="V11" si="21">R11-S11</f>
         <v>0</v>
       </c>
-      <c r="W11" s="26">
+      <c r="W11" s="23">
         <f>SUM(W3:W9)</f>
         <v>0</v>
       </c>
       <c r="X11" s="3"/>
-      <c r="Y11" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z11" s="27" t="str">
+      <c r="Y11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z11" s="24" t="str">
         <f t="shared" ref="Z11" si="22">CONCATENATE(X11, " ", Y11)</f>
         <v xml:space="preserve"> + </v>
       </c>
-      <c r="AA11" s="26">
+      <c r="AA11" s="23">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AB11" s="28">
+      <c r="AB11" s="25">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AC11" s="26">
+      <c r="AC11" s="23">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AD11" s="25">
+      <c r="AD11" s="22">
         <f t="shared" ref="AD11" si="23">IFERROR(VALUE(MID(E11,2,3)) + VALUE(MID(J11,2,3)) + VALUE(MID(O11,2,3)) + VALUE(MID(T11,2,3)) + VALUE(MID(Y11,2,3)), 0)</f>
         <v>0</v>
       </c>
-      <c r="AE11" s="27" t="str">
+      <c r="AE11" s="24" t="str">
         <f t="shared" ref="AE11" si="24">CONCATENATE(MID(AC11,1,3),"+", MID(AD11,1,2))</f>
         <v>0+0</v>
       </c>
-      <c r="AF11" s="26">
+      <c r="AF11" s="23">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -1636,65 +1631,58 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AF0419B-F030-4250-A28B-BDCB23F15824}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:AF11"/>
+  <dimension ref="A1:AA11"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="M10" activeCellId="1" sqref="Y15 M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="35" t="s">
-        <v>6</v>
-      </c>
-      <c r="X1" s="35"/>
-      <c r="Y1" s="35"/>
-      <c r="Z1" s="35"/>
-      <c r="AA1" s="35"/>
-      <c r="AB1" s="35" t="s">
+      <c r="C1" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="AC1" s="35"/>
-      <c r="AD1" s="35"/>
-      <c r="AE1" s="35"/>
-      <c r="AF1" s="35"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="7" t="s">
@@ -1754,138 +1742,106 @@
       <c r="U2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="V2" s="11" t="s">
+      <c r="V2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="W2" s="7" t="s">
+      <c r="W2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="8" t="s">
+      <c r="X2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="8" t="s">
+      <c r="Y2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="9" t="s">
+      <c r="Z2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="11" t="s">
+      <c r="AA2" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="AB2" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC2" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD2" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE2" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF2" s="15" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="7">
-        <v>1</v>
-      </c>
-      <c r="D3" s="8">
-        <v>1</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="21" t="str">
+      <c r="C3" s="7"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="19" t="str">
         <f t="shared" ref="F3:F9" si="0">SUBSTITUTE(TRIM(CONCATENATE(D3, "", E3)),"+ 0"," ")</f>
-        <v>1+ 1</v>
-      </c>
-      <c r="G3" s="22">
+        <v>+</v>
+      </c>
+      <c r="G3" s="20">
         <f>C3-D3</f>
         <v>0</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="8"/>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="21" t="str">
+      <c r="K3" s="19" t="str">
         <f t="shared" ref="K3:K9" si="1">SUBSTITUTE(TRIM(CONCATENATE(I3, "", J3)),"+ 0"," ")</f>
         <v>+</v>
       </c>
-      <c r="L3" s="22">
+      <c r="L3" s="20">
         <f>H3-I3</f>
         <v>0</v>
       </c>
       <c r="M3" s="7"/>
       <c r="N3" s="8"/>
-      <c r="O3" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="P3" s="21" t="str">
+      <c r="O3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="19" t="str">
         <f t="shared" ref="P3:P9" si="2">SUBSTITUTE(TRIM(CONCATENATE(N3, "", O3)),"+ 0"," ")</f>
         <v>+</v>
       </c>
-      <c r="Q3" s="22">
+      <c r="Q3" s="20">
         <f>M3-N3</f>
         <v>0</v>
       </c>
       <c r="R3" s="7"/>
       <c r="S3" s="8"/>
-      <c r="T3" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="U3" s="21" t="str">
+      <c r="T3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="U3" s="19" t="str">
         <f>SUBSTITUTE(TRIM(CONCATENATE(S3, "", T3)),"+ 0"," ")</f>
         <v>+</v>
       </c>
-      <c r="V3" s="23">
+      <c r="V3" s="20">
         <f>R3-S3</f>
         <v>0</v>
       </c>
-      <c r="W3" s="7"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z3" s="21" t="str">
-        <f t="shared" ref="Z3:Z9" si="3">SUBSTITUTE(TRIM(CONCATENATE(X3, "", Y3)),"+ 0"," ")</f>
-        <v>+</v>
-      </c>
-      <c r="AA3" s="23">
-        <f>W3-X3</f>
-        <v>0</v>
-      </c>
-      <c r="AB3" s="24">
-        <f t="shared" ref="AB3:AC9" si="4">C3+H3+M3+R3+W3</f>
-        <v>1</v>
-      </c>
-      <c r="AC3" s="25">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="AD3" s="25">
-        <f>IFERROR(VALUE(MID(E3,2,3)) + VALUE(MID(J3,2,3)) + VALUE(MID(O3,2,3)) + VALUE(MID(T3,2,3)) + VALUE(MID(Y3,2,3)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="AE3" s="21" t="str">
-        <f>CONCATENATE(MID(AC3,1,3)," + ", MID(AD3,1,2))</f>
-        <v>1 + 0</v>
-      </c>
-      <c r="AF3" s="23">
-        <f>G3+L3+Q3+V3+AA3</f>
+      <c r="W3" s="21">
+        <f>C3+H3+M3+R3</f>
+        <v>0</v>
+      </c>
+      <c r="X3" s="22">
+        <f>D3+I3+N3+S3</f>
+        <v>0</v>
+      </c>
+      <c r="Y3" s="22">
+        <f>IFERROR(VALUE(MID(#REF!,2,3)) + VALUE(MID(E3,2,3)) + VALUE(MID(J3,2,3)) + VALUE(MID(O3,2,3)) + VALUE(MID(T3,2,3)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z3" s="19" t="str">
+        <f>CONCATENATE(MID(X3,1,3)," + ", MID(Y3,1,2))</f>
+        <v>0 + 0</v>
+      </c>
+      <c r="AA3" s="20">
+        <f>SUM(B3,G3,L3,Q3,V3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1894,91 +1850,78 @@
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="8"/>
-      <c r="E4" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="21" t="str">
+      <c r="E4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="19" t="str">
         <f t="shared" si="0"/>
         <v>+</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="20">
         <f>C4-D4</f>
         <v>0</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="8"/>
-      <c r="J4" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="21" t="str">
+      <c r="J4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="19" t="str">
         <f t="shared" si="1"/>
         <v>+</v>
       </c>
-      <c r="L4" s="22">
+      <c r="L4" s="20">
         <f>H4-I4</f>
         <v>0</v>
       </c>
       <c r="M4" s="7"/>
       <c r="N4" s="8"/>
-      <c r="O4" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="P4" s="21" t="str">
+      <c r="O4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P4" s="19" t="str">
         <f t="shared" si="2"/>
         <v>+</v>
       </c>
-      <c r="Q4" s="22">
+      <c r="Q4" s="20">
         <f>M4-N4</f>
         <v>0</v>
       </c>
       <c r="R4" s="7"/>
       <c r="S4" s="8"/>
-      <c r="T4" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="U4" s="21" t="str">
+      <c r="T4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="U4" s="19" t="str">
         <f>SUBSTITUTE(TRIM(CONCATENATE(S4, "", T4)),"+ 0"," ")</f>
         <v>+</v>
       </c>
-      <c r="V4" s="23">
+      <c r="V4" s="20">
         <f>R4-S4</f>
         <v>0</v>
       </c>
-      <c r="W4" s="7"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z4" s="21" t="str">
-        <f t="shared" si="3"/>
-        <v>+</v>
-      </c>
-      <c r="AA4" s="23">
-        <f>W4-X4</f>
-        <v>0</v>
-      </c>
-      <c r="AB4" s="24">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AC4" s="25">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AD4" s="25">
-        <f t="shared" ref="AD4:AD11" si="5">IFERROR(VALUE(MID(E4,2,3)) + VALUE(MID(J4,2,3)) + VALUE(MID(O4,2,3)) + VALUE(MID(T4,2,3)) + VALUE(MID(Y4,2,3)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="AE4" s="21" t="str">
-        <f>CONCATENATE(MID(AC4,1,3)," + ", MID(AD4,1,2))</f>
+      <c r="W4" s="21">
+        <f t="shared" ref="W4:W9" si="3">C4+H4+M4+R4</f>
+        <v>0</v>
+      </c>
+      <c r="X4" s="22">
+        <f t="shared" ref="X4:X9" si="4">D4+I4+N4+S4</f>
+        <v>0</v>
+      </c>
+      <c r="Y4" s="22">
+        <f>IFERROR(VALUE(MID(#REF!,2,3)) + VALUE(MID(E4,2,3)) + VALUE(MID(J4,2,3)) + VALUE(MID(O4,2,3)) + VALUE(MID(T4,2,3)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z4" s="19" t="str">
+        <f>CONCATENATE(MID(X4,1,3)," + ", MID(Y4,1,2))</f>
         <v>0 + 0</v>
       </c>
-      <c r="AF4" s="23">
-        <f>G4+L4+Q4+V4+AA4</f>
+      <c r="AA4" s="20">
+        <f t="shared" ref="AA4:AA9" si="5">SUM(B4,G4,L4,Q4,V4)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1987,91 +1930,78 @@
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="21" t="str">
+      <c r="E5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="19" t="str">
         <f t="shared" si="0"/>
         <v>+</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="20">
         <f>C5-D5</f>
         <v>0</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="8"/>
-      <c r="J5" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" s="21" t="str">
+      <c r="J5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="19" t="str">
         <f t="shared" si="1"/>
         <v>+</v>
       </c>
-      <c r="L5" s="22">
+      <c r="L5" s="20">
         <f>H5-I5</f>
         <v>0</v>
       </c>
       <c r="M5" s="7"/>
       <c r="N5" s="8"/>
-      <c r="O5" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="P5" s="21" t="str">
+      <c r="O5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P5" s="19" t="str">
         <f t="shared" si="2"/>
         <v>+</v>
       </c>
-      <c r="Q5" s="22">
+      <c r="Q5" s="20">
         <f>M5-N5</f>
         <v>0</v>
       </c>
       <c r="R5" s="7"/>
       <c r="S5" s="8"/>
-      <c r="T5" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="U5" s="21" t="str">
+      <c r="T5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="U5" s="19" t="str">
         <f>SUBSTITUTE(TRIM(CONCATENATE(S5, "", T5)),"+ 0"," ")</f>
         <v>+</v>
       </c>
-      <c r="V5" s="23">
+      <c r="V5" s="20">
         <f>R5-S5</f>
         <v>0</v>
       </c>
-      <c r="W5" s="7"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z5" s="21" t="str">
+      <c r="W5" s="21">
         <f t="shared" si="3"/>
-        <v>+</v>
-      </c>
-      <c r="AA5" s="23">
-        <f>W5-X5</f>
-        <v>0</v>
-      </c>
-      <c r="AB5" s="24">
+        <v>0</v>
+      </c>
+      <c r="X5" s="22">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AC5" s="25">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AD5" s="25">
+      <c r="Y5" s="22">
+        <f>IFERROR(VALUE(MID(#REF!,2,3)) + VALUE(MID(E5,2,3)) + VALUE(MID(J5,2,3)) + VALUE(MID(O5,2,3)) + VALUE(MID(T5,2,3)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z5" s="19" t="str">
+        <f>CONCATENATE(MID(X5,1,3)," + ", MID(Y5,1,2))</f>
+        <v>0 + 0</v>
+      </c>
+      <c r="AA5" s="20">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AE5" s="21" t="str">
-        <f>CONCATENATE(MID(AC5,1,3)," + ", MID(AD5,1,2))</f>
-        <v>0 + 0</v>
-      </c>
-      <c r="AF5" s="23">
-        <f>G5+L5+Q5+V5+AA5</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2080,91 +2010,78 @@
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="8"/>
-      <c r="E6" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="21" t="str">
+      <c r="E6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="19" t="str">
         <f t="shared" si="0"/>
         <v>+</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="20">
         <f>C6-D6</f>
         <v>0</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="8"/>
-      <c r="J6" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="K6" s="21" t="str">
+      <c r="J6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="19" t="str">
         <f t="shared" si="1"/>
         <v>+</v>
       </c>
-      <c r="L6" s="22">
+      <c r="L6" s="20">
         <f>H6-I6</f>
         <v>0</v>
       </c>
       <c r="M6" s="7"/>
       <c r="N6" s="8"/>
-      <c r="O6" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="P6" s="21" t="str">
+      <c r="O6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P6" s="19" t="str">
         <f t="shared" si="2"/>
         <v>+</v>
       </c>
-      <c r="Q6" s="22">
+      <c r="Q6" s="20">
         <f>M6-N6</f>
         <v>0</v>
       </c>
       <c r="R6" s="7"/>
       <c r="S6" s="8"/>
-      <c r="T6" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="U6" s="21" t="str">
+      <c r="T6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="U6" s="19" t="str">
         <f>SUBSTITUTE(TRIM(CONCATENATE(S6, "", T6)),"+ 0"," ")</f>
         <v>+</v>
       </c>
-      <c r="V6" s="23">
+      <c r="V6" s="20">
         <f>R6-S6</f>
         <v>0</v>
       </c>
-      <c r="W6" s="7"/>
-      <c r="X6" s="8"/>
-      <c r="Y6" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z6" s="21" t="str">
+      <c r="W6" s="21">
         <f t="shared" si="3"/>
-        <v>+</v>
-      </c>
-      <c r="AA6" s="23">
-        <f>W6-X6</f>
-        <v>0</v>
-      </c>
-      <c r="AB6" s="24">
-        <f>C6+H6+M6+R6+W6</f>
-        <v>0</v>
-      </c>
-      <c r="AC6" s="25">
+        <v>0</v>
+      </c>
+      <c r="X6" s="22">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AD6" s="25">
+      <c r="Y6" s="22">
+        <f>IFERROR(VALUE(MID(#REF!,2,3)) + VALUE(MID(E6,2,3)) + VALUE(MID(J6,2,3)) + VALUE(MID(O6,2,3)) + VALUE(MID(T6,2,3)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z6" s="19" t="str">
+        <f>CONCATENATE(MID(X6,1,3)," + ", MID(Y6,1,2))</f>
+        <v>0 + 0</v>
+      </c>
+      <c r="AA6" s="20">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AE6" s="21" t="str">
-        <f>CONCATENATE(MID(AC6,1,3)," + ", MID(AD6,1,2))</f>
-        <v>0 + 0</v>
-      </c>
-      <c r="AF6" s="23">
-        <f>G6+L6+Q6+V6+AA6</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2173,91 +2090,78 @@
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="21" t="str">
+      <c r="E7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="19" t="str">
         <f t="shared" si="0"/>
         <v>+</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="20">
         <f>C7-D7</f>
         <v>0</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="8"/>
-      <c r="J7" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="21" t="str">
+      <c r="J7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="19" t="str">
         <f t="shared" si="1"/>
         <v>+</v>
       </c>
-      <c r="L7" s="22">
+      <c r="L7" s="20">
         <f>H7-I7</f>
         <v>0</v>
       </c>
       <c r="M7" s="7"/>
       <c r="N7" s="8"/>
-      <c r="O7" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="P7" s="21" t="str">
+      <c r="O7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P7" s="19" t="str">
         <f t="shared" si="2"/>
         <v>+</v>
       </c>
-      <c r="Q7" s="22">
+      <c r="Q7" s="20">
         <f>M7-N7</f>
         <v>0</v>
       </c>
       <c r="R7" s="7"/>
       <c r="S7" s="8"/>
-      <c r="T7" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="U7" s="21" t="str">
+      <c r="T7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="U7" s="19" t="str">
         <f>SUBSTITUTE(TRIM(CONCATENATE(S7, "", T7)),"+ 0"," ")</f>
         <v>+</v>
       </c>
-      <c r="V7" s="23">
+      <c r="V7" s="20">
         <f>R7-S7</f>
         <v>0</v>
       </c>
-      <c r="W7" s="7"/>
-      <c r="X7" s="8"/>
-      <c r="Y7" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z7" s="21" t="str">
+      <c r="W7" s="21">
         <f t="shared" si="3"/>
-        <v>+</v>
-      </c>
-      <c r="AA7" s="23">
-        <f>W7-X7</f>
-        <v>0</v>
-      </c>
-      <c r="AB7" s="24">
-        <f>C7+H7+M7+R7+W7</f>
-        <v>0</v>
-      </c>
-      <c r="AC7" s="25">
+        <v>0</v>
+      </c>
+      <c r="X7" s="22">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AD7" s="25">
+      <c r="Y7" s="22">
+        <f>IFERROR(VALUE(MID(#REF!,2,3)) + VALUE(MID(E7,2,3)) + VALUE(MID(J7,2,3)) + VALUE(MID(O7,2,3)) + VALUE(MID(T7,2,3)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z7" s="19" t="str">
+        <f>CONCATENATE(MID(X7,1,3)," + ", MID(Y7,1,2))</f>
+        <v>0 + 0</v>
+      </c>
+      <c r="AA7" s="20">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AE7" s="21" t="str">
-        <f>CONCATENATE(MID(AC7,1,3)," + ", MID(AD7,1,2))</f>
-        <v>0 + 0</v>
-      </c>
-      <c r="AF7" s="23">
-        <f>G7+L7+Q7+V7+AA7</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2266,327 +2170,279 @@
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="8"/>
-      <c r="E8" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="21" t="str">
+      <c r="E8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="19" t="str">
         <f t="shared" si="0"/>
         <v>+</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G8" s="20">
         <f t="shared" ref="G8:G9" si="6">C8-D8</f>
         <v>0</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="8"/>
-      <c r="J8" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" s="21" t="str">
+      <c r="J8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="19" t="str">
         <f t="shared" si="1"/>
         <v>+</v>
       </c>
-      <c r="L8" s="22">
+      <c r="L8" s="20">
         <f t="shared" ref="L8:L9" si="7">H8-I8</f>
         <v>0</v>
       </c>
       <c r="M8" s="7"/>
       <c r="N8" s="8"/>
-      <c r="O8" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="P8" s="21" t="str">
+      <c r="O8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P8" s="19" t="str">
         <f t="shared" si="2"/>
         <v>+</v>
       </c>
-      <c r="Q8" s="22">
+      <c r="Q8" s="20">
         <f t="shared" ref="Q8:Q9" si="8">M8-N8</f>
         <v>0</v>
       </c>
       <c r="R8" s="7"/>
       <c r="S8" s="8"/>
-      <c r="T8" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="U8" s="21" t="str">
+      <c r="T8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="U8" s="19" t="str">
         <f t="shared" ref="U8:U9" si="9">SUBSTITUTE(TRIM(CONCATENATE(S8, "", T8)),"+ 0"," ")</f>
         <v>+</v>
       </c>
-      <c r="V8" s="23">
+      <c r="V8" s="20">
         <f t="shared" ref="V8:V9" si="10">R8-S8</f>
         <v>0</v>
       </c>
-      <c r="W8" s="7"/>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z8" s="21" t="str">
+      <c r="W8" s="21">
         <f t="shared" si="3"/>
-        <v>+</v>
-      </c>
-      <c r="AA8" s="23">
-        <f t="shared" ref="AA8:AA11" si="11">W8-X8</f>
-        <v>0</v>
-      </c>
-      <c r="AB8" s="24">
-        <f t="shared" ref="AB8:AC11" si="12">C8+H8+M8+R8+W8</f>
-        <v>0</v>
-      </c>
-      <c r="AC8" s="25">
+        <v>0</v>
+      </c>
+      <c r="X8" s="22">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AD8" s="25">
+      <c r="Y8" s="22">
+        <f>IFERROR(VALUE(MID(#REF!,2,3)) + VALUE(MID(E8,2,3)) + VALUE(MID(J8,2,3)) + VALUE(MID(O8,2,3)) + VALUE(MID(T8,2,3)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z8" s="19" t="str">
+        <f t="shared" ref="Z8:Z9" si="11">CONCATENATE(MID(X8,1,3)," + ", MID(Y8,1,2))</f>
+        <v>0 + 0</v>
+      </c>
+      <c r="AA8" s="20">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AE8" s="21" t="str">
-        <f t="shared" ref="AE8:AE9" si="13">CONCATENATE(MID(AC8,1,3)," + ", MID(AD8,1,2))</f>
-        <v>0 + 0</v>
-      </c>
-      <c r="AF8" s="23">
-        <f t="shared" ref="AF8:AF11" si="14">G8+L8+Q8+V8+AA8</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="21" t="str">
+      <c r="E9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="19" t="str">
         <f t="shared" si="0"/>
         <v>+</v>
       </c>
-      <c r="G9" s="22">
+      <c r="G9" s="20">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="8"/>
-      <c r="J9" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="K9" s="21" t="str">
+      <c r="J9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="19" t="str">
         <f t="shared" si="1"/>
         <v>+</v>
       </c>
-      <c r="L9" s="22">
+      <c r="L9" s="20">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M9" s="7"/>
       <c r="N9" s="8"/>
-      <c r="O9" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="P9" s="21" t="str">
+      <c r="O9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P9" s="19" t="str">
         <f t="shared" si="2"/>
         <v>+</v>
       </c>
-      <c r="Q9" s="22">
+      <c r="Q9" s="20">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="R9" s="7"/>
       <c r="S9" s="8"/>
-      <c r="T9" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="U9" s="21" t="str">
+      <c r="T9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="U9" s="19" t="str">
         <f t="shared" si="9"/>
         <v>+</v>
       </c>
-      <c r="V9" s="23">
+      <c r="V9" s="20">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="W9" s="7"/>
-      <c r="X9" s="8"/>
-      <c r="Y9" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z9" s="21" t="str">
+      <c r="W9" s="21">
         <f t="shared" si="3"/>
-        <v>+</v>
-      </c>
-      <c r="AA9" s="23">
+        <v>0</v>
+      </c>
+      <c r="X9" s="22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Y9" s="22">
+        <f>IFERROR(VALUE(MID(#REF!,2,3)) + VALUE(MID(E9,2,3)) + VALUE(MID(J9,2,3)) + VALUE(MID(O9,2,3)) + VALUE(MID(T9,2,3)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z9" s="19" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AB9" s="24">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AC9" s="25">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AD9" s="25">
+        <v>0 + 0</v>
+      </c>
+      <c r="AA9" s="20">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AE9" s="21" t="str">
-        <f t="shared" si="13"/>
-        <v>0 + 0</v>
-      </c>
-      <c r="AF9" s="23">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="16"/>
+      <c r="E10" s="14"/>
       <c r="F10" s="9"/>
       <c r="G10" s="10"/>
       <c r="H10" s="7"/>
       <c r="I10" s="8"/>
-      <c r="J10" s="16"/>
+      <c r="J10" s="14"/>
       <c r="K10" s="9"/>
       <c r="L10" s="10"/>
       <c r="M10" s="7"/>
       <c r="N10" s="8"/>
-      <c r="O10" s="16"/>
+      <c r="O10" s="14"/>
       <c r="P10" s="9"/>
       <c r="Q10" s="10"/>
       <c r="R10" s="7"/>
       <c r="S10" s="8"/>
-      <c r="T10" s="16"/>
+      <c r="T10" s="14"/>
       <c r="U10" s="9"/>
-      <c r="V10" s="11"/>
-      <c r="W10" s="7"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="15"/>
       <c r="X10" s="8"/>
-      <c r="Y10" s="16"/>
+      <c r="Y10" s="8"/>
       <c r="Z10" s="9"/>
-      <c r="AA10" s="11"/>
-      <c r="AB10" s="17"/>
-      <c r="AC10" s="8"/>
-      <c r="AD10" s="8"/>
-      <c r="AE10" s="9"/>
-      <c r="AF10" s="11"/>
+      <c r="AA10" s="10"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A11" s="18" t="s">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="26">
+      <c r="B11" s="17"/>
+      <c r="C11" s="23">
         <f>SUM(C3:C9)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" s="3"/>
-      <c r="E11" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="27" t="str">
-        <f t="shared" ref="F11" si="15">CONCATENATE(D11, " ", E11)</f>
+      <c r="E11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="24" t="str">
+        <f t="shared" ref="F11" si="12">CONCATENATE(D11, " ", E11)</f>
         <v xml:space="preserve"> + </v>
       </c>
-      <c r="G11" s="26">
+      <c r="G11" s="23">
         <f>C11-D11</f>
-        <v>1</v>
-      </c>
-      <c r="H11" s="26">
+        <v>0</v>
+      </c>
+      <c r="H11" s="23">
         <f>SUM(H3:H9)</f>
         <v>0</v>
       </c>
       <c r="I11" s="3"/>
-      <c r="J11" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="27" t="str">
-        <f t="shared" ref="K11" si="16">CONCATENATE(I11, " ", J11)</f>
+      <c r="J11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="24" t="str">
+        <f t="shared" ref="K11" si="13">CONCATENATE(I11, " ", J11)</f>
         <v xml:space="preserve"> + </v>
       </c>
-      <c r="L11" s="26">
-        <f t="shared" ref="L11" si="17">H11-I11</f>
-        <v>0</v>
-      </c>
-      <c r="M11" s="26">
+      <c r="L11" s="23">
+        <f t="shared" ref="L11" si="14">H11-I11</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="23">
         <f>SUM(M3:M9)</f>
         <v>0</v>
       </c>
       <c r="N11" s="3"/>
-      <c r="O11" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="P11" s="27" t="str">
-        <f t="shared" ref="P11" si="18">CONCATENATE(N11, " ", O11)</f>
+      <c r="O11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="P11" s="24" t="str">
+        <f t="shared" ref="P11" si="15">CONCATENATE(N11, " ", O11)</f>
         <v xml:space="preserve"> + </v>
       </c>
-      <c r="Q11" s="26">
-        <f t="shared" ref="Q11" si="19">M11-N11</f>
-        <v>0</v>
-      </c>
-      <c r="R11" s="26">
+      <c r="Q11" s="23">
+        <f t="shared" ref="Q11" si="16">M11-N11</f>
+        <v>0</v>
+      </c>
+      <c r="R11" s="23">
         <f>SUM(R3:R9)</f>
         <v>0</v>
       </c>
       <c r="S11" s="3"/>
-      <c r="T11" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="U11" s="27" t="str">
-        <f t="shared" ref="U11" si="20">CONCATENATE(S11, "", T11)</f>
+      <c r="T11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="U11" s="24" t="str">
+        <f t="shared" ref="U11" si="17">CONCATENATE(S11, "", T11)</f>
         <v xml:space="preserve">+ </v>
       </c>
-      <c r="V11" s="26">
-        <f t="shared" ref="V11" si="21">R11-S11</f>
-        <v>0</v>
-      </c>
-      <c r="W11" s="26">
-        <f>SUM(W3:W9)</f>
-        <v>0</v>
-      </c>
-      <c r="X11" s="3"/>
-      <c r="Y11" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z11" s="27" t="str">
-        <f t="shared" ref="Z11" si="22">CONCATENATE(X11, " ", Y11)</f>
-        <v xml:space="preserve"> + </v>
-      </c>
-      <c r="AA11" s="26">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AB11" s="28">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="AC11" s="26">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD11" s="25">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AE11" s="27" t="str">
-        <f t="shared" ref="AE11" si="23">CONCATENATE(MID(AC11,1,3),"+", MID(AD11,1,2))</f>
+      <c r="V11" s="23">
+        <f t="shared" ref="V11" si="18">R11-S11</f>
+        <v>0</v>
+      </c>
+      <c r="W11" s="25">
+        <f>C11+H11+M11+R11</f>
+        <v>0</v>
+      </c>
+      <c r="X11" s="23">
+        <f>D11+I11+N11+S11</f>
+        <v>0</v>
+      </c>
+      <c r="Y11" s="22">
+        <f>IFERROR(VALUE(MID(#REF!,2,3)) + VALUE(MID(E11,2,3)) + VALUE(MID(J11,2,3)) + VALUE(MID(O11,2,3)) + VALUE(MID(T11,2,3)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z11" s="24" t="str">
+        <f t="shared" ref="Z11" si="19">CONCATENATE(MID(X11,1,3),"+", MID(Y11,1,2))</f>
         <v>0+0</v>
       </c>
-      <c r="AF11" s="26">
-        <f t="shared" si="14"/>
-        <v>1</v>
+      <c r="AA11" s="23">
+        <f>B11+G11+L11+Q11+V11</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
-  <mergeCells count="6">
-    <mergeCell ref="AB1:AF1"/>
+  <sheetProtection sheet="1" selectLockedCells="1"/>
+  <mergeCells count="5">
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="H1:L1"/>
     <mergeCell ref="M1:Q1"/>

</xml_diff>